<commit_message>
0327 edit all feedback
</commit_message>
<xml_diff>
--- a/DataTable/FarmerLevelupGoldTable.xlsx
+++ b/DataTable/FarmerLevelupGoldTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fc6ad1120df1f34/문서/GitHub/ProjectF/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E9EFC4-905E-CB4F-9C00-CEAED15FB19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{51E9EFC4-905E-CB4F-9C00-CEAED15FB19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4C67419-DB9A-40C3-95B0-D986DA22E80B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="29040" windowHeight="15720" xr2:uid="{6D834648-F0A2-4D19-9C67-DDF58A439875}"/>
+    <workbookView xWindow="5040" yWindow="2640" windowWidth="21615" windowHeight="11295" xr2:uid="{6D834648-F0A2-4D19-9C67-DDF58A439875}"/>
   </bookViews>
   <sheets>
     <sheet name="FarmerLevelupGoldTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -48,55 +48,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CommonBaseValue</t>
+    <t>Erarity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UnCommonBaseValue</t>
+    <t>Common</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RareBaseValue</t>
+    <t>UnCommon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EpicBaseValue</t>
+    <t>Rare</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LegendaryBaseValue</t>
+    <t>Epic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MythicBaseValue</t>
+    <t>Legendary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CommonMultiplierValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UnCommonMultiplierValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RareMultiplierValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EpicMultiplierValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LegendaryMultiplierValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MythicMultiplierValue</t>
+    <t>Mythic</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiplierValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,8 +126,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -144,14 +142,381 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -166,7 +531,22 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
@@ -175,7 +555,63 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
@@ -184,7 +620,7 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -199,33 +635,22 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -235,26 +660,131 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -272,6 +802,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,151 +1125,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E233CD0-531C-46D3-82AC-F946B166DEB6}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:AY12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
+    <col min="7" max="7" width="15.625" customWidth="1"/>
     <col min="8" max="8" width="22.5" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="17.5" customWidth="1"/>
     <col min="12" max="12" width="22.5" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" customWidth="1"/>
+    <col min="13" max="13" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1"/>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:51" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="5"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="7"/>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="8"/>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="10"/>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A4" s="35">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="36">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="30"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A5" s="35">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="37">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F5" s="25"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A6" s="35">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="36">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A7" s="35">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="37">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="A8" s="35">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="36">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="9" spans="1:51" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="38">
+        <v>5</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="39">
+        <v>6</v>
+      </c>
+      <c r="D9" s="40">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" ht="18" thickBot="1">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>15</v>
-      </c>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="F10" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="18" thickBot="1">
-      <c r="A4" s="5">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>50</v>
-      </c>
-      <c r="C4" s="6">
-        <v>75</v>
-      </c>
-      <c r="D4" s="6">
-        <v>100</v>
-      </c>
-      <c r="E4" s="6">
-        <v>150</v>
-      </c>
-      <c r="F4" s="6">
-        <v>200</v>
-      </c>
-      <c r="G4" s="6">
-        <v>300</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1.3</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1.7</v>
-      </c>
-      <c r="L4" s="6">
-        <v>2</v>
-      </c>
-      <c r="M4" s="6">
-        <v>2.5</v>
-      </c>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>